<commit_message>
new content to publish
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-Humancoronavirus229ERNAPrThrPtNphOrdNonprobeamptarLabObs.xlsx
+++ b/output/StructureDefinition-Humancoronavirus229ERNAPrThrPtNphOrdNonprobeamptarLabObs.xlsx
@@ -1755,15 +1755,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="43.6015625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="43.60546875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="37.0" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="66.26953125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1776,13 +1776,13 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.56640625" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="68.40625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="27.84765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="27.8515625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>

</xml_diff>

<commit_message>
Fresh source restore from fsh branch.
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-Humancoronavirus229ERNAPrThrPtNphOrdNonprobeamptarLabObs.xlsx
+++ b/output/StructureDefinition-Humancoronavirus229ERNAPrThrPtNphOrdNonprobeamptarLabObs.xlsx
@@ -1755,15 +1755,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="43.6015625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="43.60546875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="37.0" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="66.26953125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1776,13 +1776,13 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.56640625" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="68.40625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="27.84765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="27.8515625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>

</xml_diff>